<commit_message>
feat: Complete transport reports system with modal-based creation and display functionality
- Added CreateTransportReportModal for clean form interface
- Added TransportReportsList with search and filtering
- Added ViewTransportReportModal for detailed report viewing
- Updated API routes to save reports to database
- Added frontend services and hooks for state management
- Implemented real-time status functionality
- Updated database schema and types
- Added comprehensive error handling and validation
- Improved UI/UX with responsive design and loading states
</commit_message>
<xml_diff>
--- a/flight_info.xlsx
+++ b/flight_info.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -40,13 +40,16 @@
     <t xml:space="preserve">Property Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Vehicle Standby</t>
+    <t xml:space="preserve">Vehicle Standby Arrival</t>
   </si>
   <si>
     <t xml:space="preserve">Departure Date</t>
   </si>
   <si>
     <t xml:space="preserve">Departure Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehicle Standby Departure</t>
   </si>
   <si>
     <t xml:space="preserve">Status</t>
@@ -470,8 +473,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -514,21 +517,21 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>45861</v>
@@ -537,7 +540,7 @@
         <v>0.96875</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" s="8" t="n">
         <v>0.875</v>
@@ -552,18 +555,18 @@
         <v>0.524305555555556</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="12" t="n">
         <v>45860</v>
@@ -572,7 +575,7 @@
         <v>0.694444444444444</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="13" t="n">
         <v>0.635416666666667</v>
@@ -587,18 +590,18 @@
         <v>0.364583333333333</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>45861</v>
@@ -607,7 +610,7 @@
         <v>0.96875</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="8" t="n">
         <v>0.875</v>
@@ -622,18 +625,18 @@
         <v>0.524305555555556</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D5" s="12" t="n">
         <v>45859</v>
@@ -642,7 +645,7 @@
         <v>0.138888888888889</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" s="13" t="n">
         <v>0.0416666666666667</v>
@@ -657,18 +660,18 @@
         <v>0.166666666666667</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="12" t="n">
         <v>45861</v>
@@ -677,7 +680,7 @@
         <v>0.784722222222222</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" s="13" t="n">
         <v>0.708333333333333</v>
@@ -692,18 +695,18 @@
         <v>0.395833333333333</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D7" s="12" t="n">
         <v>45863</v>
@@ -712,7 +715,7 @@
         <v>0.850694444444444</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G7" s="13" t="n">
         <v>0.78125</v>
@@ -727,10 +730,10 @@
         <v>0.569444444444444</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>

</xml_diff>